<commit_message>
Add SourceIndex tracking and update_valeur_origine function
Co-authored-by: alainthiebaud <210218067+alainthiebaud@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/assets/frais_divers_annuels.xlsx
+++ b/assets/frais_divers_annuels.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Administration" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Assurances" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Taxes" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="frais divers" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -456,7 +457,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="3">
@@ -748,275 +749,349 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FB572CDC1A90BC4B93BA4B2927B30705" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="2268db72fa954f1a3801c90b31d73c03">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9bdf6784-7464-4893-ac02-5c6d253a4184" xmlns:ns3="379d16dd-8fb1-4211-866b-4b68628b155e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8ef11724ad7eb63881d1916f0cda64d0" ns2:_="" ns3:_="">
-    <xsd:import namespace="9bdf6784-7464-4893-ac02-5c6d253a4184"/>
-    <xsd:import namespace="379d16dd-8fb1-4211-866b-4b68628b155e"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9bdf6784-7464-4893-ac02-5c6d253a4184" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="11" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="13" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="20" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="a653a3c4-7aab-42c9-bca9-c23808d1d478" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="22" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="23" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="379d16dd-8fb1-4211-866b-4b68628b155e" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="17" nillable="true" ma:displayName="Partagé avec" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="18" nillable="true" ma:displayName="Partagé avec détails" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="21" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{ae647290-a933-43f1-b10f-c781fe5414b4}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="379d16dd-8fb1-4211-866b-4b68628b155e">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Type de contenu"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titre"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9bdf6784-7464-4893-ac02-5c6d253a4184">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="379d16dd-8fb1-4211-866b-4b68628b155e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DEC1914-1749-4248-9937-899BCD53343F}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CB2D14C-01F3-4F5D-B280-F4CEF9FC4001}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F65E23-1A5F-4378-8496-025A60DFC645}"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Montant (CHF)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Groupe</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>SourceIndex</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Salaire et charges sociales du concierge</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Entretien</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Contrat entreprise de nettoyage</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Entretien</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Produits de nettoyage et petit matériel</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Entretien</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Entretien du jardin / espaces verts</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>600</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Entretien</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Service de déneigement</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Entretien</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Salaire et charges sociales du concierge</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1200</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Entretien</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Contrat de service de l'ascenseur</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>3000</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Maintenance</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Contrat d'entretien du chauffage (PAC/Chaudière)</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>800</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Maintenance</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Entretien des machines de buanderie</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Maintenance</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Maintenance porte de garage</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Maintenance</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Contrôle des extincteurs</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Maintenance</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Frais de ramonage / contrôle officiel</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Maintenance</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Honoraires de gérance / administration</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>600</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Administration</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Frais de compte bancaire de l'immeuble</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Administration</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Assurance bâtiment (ECA)</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Assurances</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Assurance RC de l'immeuble</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Assurances</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Taxe d'enlèvement des ordures</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Taxes</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement hierarchical TreeView and editing for Frais divers
Co-authored-by: alainthiebaud <210218067+alainthiebaud@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/assets/frais_divers_annuels.xlsx
+++ b/assets/frais_divers_annuels.xlsx
@@ -453,11 +453,13 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Salaire et charges sociales du concierge</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>1000</v>
+          <t>Modified Description</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -792,7 +794,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Complete implementation of Frais divers hierarchical editing with documentation
Co-authored-by: alainthiebaud <210218067+alainthiebaud@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/assets/frais_divers_annuels.xlsx
+++ b/assets/frais_divers_annuels.xlsx
@@ -456,10 +456,8 @@
           <t>Modified Description</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2024-01-15</t>
-        </is>
+      <c r="B2" t="n">
+        <v>2500</v>
       </c>
     </row>
     <row r="3">
@@ -469,7 +467,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>750</v>
       </c>
     </row>
     <row r="4">
@@ -546,7 +544,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Contrat de service de l'ascenseur</t>
+          <t>Modified by SourceIndex test</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -790,11 +788,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Salaire et charges sociales du concierge</t>
+          <t>Modified Description</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1500</v>
+        <v>2500</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -812,7 +810,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -898,7 +896,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Contrat de service de l'ascenseur</t>
+          <t>Modified by SourceIndex test</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>

<commit_message>
Implement hierarchical display for Frais divers tab
Co-authored-by: alainthiebaud <210218067+alainthiebaud@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/assets/frais_divers_annuels.xlsx
+++ b/assets/frais_divers_annuels.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Administration" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Assurances" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Taxes" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="frais divers" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -748,275 +749,293 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FB572CDC1A90BC4B93BA4B2927B30705" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="2268db72fa954f1a3801c90b31d73c03">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9bdf6784-7464-4893-ac02-5c6d253a4184" xmlns:ns3="379d16dd-8fb1-4211-866b-4b68628b155e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8ef11724ad7eb63881d1916f0cda64d0" ns2:_="" ns3:_="">
-    <xsd:import namespace="9bdf6784-7464-4893-ac02-5c6d253a4184"/>
-    <xsd:import namespace="379d16dd-8fb1-4211-866b-4b68628b155e"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9bdf6784-7464-4893-ac02-5c6d253a4184" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="11" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="13" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="20" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="a653a3c4-7aab-42c9-bca9-c23808d1d478" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="22" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="23" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="379d16dd-8fb1-4211-866b-4b68628b155e" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="17" nillable="true" ma:displayName="Partagé avec" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="18" nillable="true" ma:displayName="Partagé avec détails" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="21" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{ae647290-a933-43f1-b10f-c781fe5414b4}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="379d16dd-8fb1-4211-866b-4b68628b155e">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Type de contenu"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titre"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9bdf6784-7464-4893-ac02-5c6d253a4184">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="379d16dd-8fb1-4211-866b-4b68628b155e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DEC1914-1749-4248-9937-899BCD53343F}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CB2D14C-01F3-4F5D-B280-F4CEF9FC4001}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F65E23-1A5F-4378-8496-025A60DFC645}"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Montant (CHF)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Groupe</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Frais de compte bancaire de l'immeuble</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Administration</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Honoraires de gérance / administration</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>600</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Administration</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Assurance RC de l'immeuble</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Assurances</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Assurance bâtiment (ECA)</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Assurances</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Contrat entreprise de nettoyage</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Entretien</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Entretien du jardin / espaces verts</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>600</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Entretien</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Produits de nettoyage et petit matériel</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Entretien</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Salaire et charges sociales du concierge</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Entretien</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Salaire et charges sociales du concierge</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1200</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Entretien</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Service de déneigement</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Entretien</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Contrat d'entretien du chauffage (PAC/Chaudière)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>800</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Maintenance</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Contrat de service de l'ascenseur</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>3000</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Maintenance</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Contrôle des extincteurs</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Maintenance</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Entretien des machines de buanderie</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Maintenance</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Frais de ramonage / contrôle officiel</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Maintenance</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Maintenance porte de garage</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Maintenance</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Taxe d'enlèvement des ordures</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Taxes</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Complete hierarchical display implementation with add/delete functionality
Co-authored-by: alainthiebaud <210218067+alainthiebaud@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/assets/frais_divers_annuels.xlsx
+++ b/assets/frais_divers_annuels.xlsx
@@ -755,7 +755,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1035,6 +1035,21 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Test item added programmatically</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>123.45</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Entretien</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Description de la modification
</commit_message>
<xml_diff>
--- a/assets/frais_divers_annuels.xlsx
+++ b/assets/frais_divers_annuels.xlsx
@@ -1053,4 +1053,277 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FB572CDC1A90BC4B93BA4B2927B30705" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="2268db72fa954f1a3801c90b31d73c03">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9bdf6784-7464-4893-ac02-5c6d253a4184" xmlns:ns3="379d16dd-8fb1-4211-866b-4b68628b155e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8ef11724ad7eb63881d1916f0cda64d0" ns2:_="" ns3:_="">
+    <xsd:import namespace="9bdf6784-7464-4893-ac02-5c6d253a4184"/>
+    <xsd:import namespace="379d16dd-8fb1-4211-866b-4b68628b155e"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9bdf6784-7464-4893-ac02-5c6d253a4184" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="11" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="13" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="20" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="a653a3c4-7aab-42c9-bca9-c23808d1d478" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="22" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="23" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="379d16dd-8fb1-4211-866b-4b68628b155e" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="17" nillable="true" ma:displayName="Partagé avec" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="18" nillable="true" ma:displayName="Partagé avec détails" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="21" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{ae647290-a933-43f1-b10f-c781fe5414b4}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="379d16dd-8fb1-4211-866b-4b68628b155e">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Type de contenu"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titre"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9bdf6784-7464-4893-ac02-5c6d253a4184">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="379d16dd-8fb1-4211-866b-4b68628b155e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{949BDD2C-9607-400B-8690-567D1DAE58DB}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB939CD4-B0EB-4A7B-9CBC-01CD7B46F5B8}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3FBCD0A-30A2-4407-9E1C-7901EB5A0745}"/>
 </file>
</xml_diff>